<commit_message>
added condensed table - dependent on uniform skus as well as the rest of the ProFocus websites.
</commit_message>
<xml_diff>
--- a/Piviot_table_example.xlsx
+++ b/Piviot_table_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sam/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sam/Desktop/Epson_WS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E9CE81-2229-D041-AC5E-EC0A22B6C6B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BA4091-4D10-4947-8F7E-993F6E3A3953}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="16480" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="3200" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -9374,7 +9374,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:N26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" showAll="0">
@@ -27560,7 +27560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>

</xml_diff>